<commit_message>
Excel Write issue corrected, folder structure re organized, added few more look and feel
</commit_message>
<xml_diff>
--- a/RootCauseAnalyzer/uploaded_defects.xlsx
+++ b/RootCauseAnalyzer/uploaded_defects.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Moumita\Delay data\RCA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\392915\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36208E81-86F3-4259-924A-FB751776EB8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95EEFC8-0BD3-44FD-978E-E5CA38E62D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{5F85C9A7-D03E-496D-8BA1-A718B27A219A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{762458F1-1140-4D8C-B786-3D5760936ED4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="All Incidents_Mar'24" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All Incidents_Mar''24'!$A$1:$X$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>IncidentID</t>
   </si>
@@ -76,67 +79,13 @@
   </si>
   <si>
     <t>StatusDescription</t>
-  </si>
-  <si>
-    <t>2402139</t>
-  </si>
-  <si>
-    <t>iCargo Payment Portal</t>
-  </si>
-  <si>
-    <t>User trying to use Alaska Payments from Citrix but gets a black screen now earlier was getting an error about a virus</t>
-  </si>
-  <si>
-    <t>ITS Airport Operations</t>
-  </si>
-  <si>
-    <t>Enterprise Applications</t>
-  </si>
-  <si>
-    <t>Closed</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Advice &amp; Guidance</t>
-  </si>
-  <si>
-    <t>User was able to take cargo payments after guidance on refreshing application if it shows a blank screen.</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Incident is closed</t>
-  </si>
-  <si>
-    <t>2420660</t>
-  </si>
-  <si>
-    <t>iCargo Application Software</t>
-  </si>
-  <si>
-    <t>iCargo system running extremely slow, causing heavy backups.</t>
-  </si>
-  <si>
-    <t>Portal</t>
-  </si>
-  <si>
-    <t>Seems to have been an issue with the iCargo network. Please re-create a ticket if issue reoccurs.</t>
-  </si>
-  <si>
-    <t>06/19 | SEAFF | BRF | iCargo system running extremely slow., causing heavy backups.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,16 +93,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -161,12 +124,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -185,9 +165,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -225,7 +205,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -331,7 +311,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -473,153 +453,82 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39017C2-AE50-4C4D-9A80-7CD4231E91F5}">
-  <dimension ref="A1:N3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BBEDB6-7FC7-4D1A-9DA6-4588835ACBB4}">
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048404"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1796875" customWidth="1"/>
+    <col min="4" max="4" width="32.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.6328125" customWidth="1"/>
+    <col min="10" max="10" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3">
-        <v>7</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" t="s">
-        <v>25</v>
-      </c>
+      <c r="O1" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>